<commit_message>
lab_02 and lab_03 fix mistakes ГОСТ
</commit_message>
<xml_diff>
--- a/lab_02/docs/csv/time.xlsx
+++ b/lab_02/docs/csv/time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Analiz_Algorith\lab_02\docs\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FCEA29-FC02-47B4-8052-3C79360B6A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709ABA8E-44D8-4328-BC2B-EDE0901F349D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="even" sheetId="1" r:id="rId1"/>
@@ -499,11 +499,15 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t> NxN</a:t>
+                  <a:t>,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
-                  <a:t> </a:t>
+                  <a:t>кол-во элементов </a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU"/>
               </a:p>
@@ -1171,15 +1175,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Размер матрицы</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t> NxN</a:t>
+                  <a:t>Размер матрицы,</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
-                  <a:t> </a:t>
+                  <a:t> кол-во элементов </a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU"/>
               </a:p>
@@ -2927,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:D11"/>
+    <sheetView topLeftCell="C1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408492EB-73D2-4BE5-AF5C-90D8072413EB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>